<commit_message>
Se añadieron seleccion de proyectos
</commit_message>
<xml_diff>
--- a/uploads/metricas_2025-07.xlsx
+++ b/uploads/metricas_2025-07.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AROBLEDO\Downloads\Dashboard Agosto\SonarQube (1)\SonarQube\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arg_2\OneDrive\Escritorio\Dashboard\SonarQube\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFFEF26-9CDC-4B23-A98C-9BDDFF749C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA532DE-651F-4268-BB67-EF18B7E4291F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="384" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$393</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$394</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1892,9 +1892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N394"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A394" sqref="A394"/>
     </sheetView>
   </sheetViews>
@@ -1954,7 +1955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2065,7 +2066,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2109,7 +2110,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2153,7 +2154,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2241,7 +2242,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2314,7 +2315,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2490,7 +2491,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -2534,7 +2535,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2578,7 +2579,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2604,7 +2605,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -2780,7 +2781,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2824,7 +2825,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2868,7 +2869,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2906,7 +2907,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -2994,7 +2995,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -3082,7 +3083,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -3167,7 +3168,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -3211,7 +3212,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -3237,7 +3238,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -3325,7 +3326,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -3366,7 +3367,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -3410,7 +3411,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -3451,7 +3452,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -3492,7 +3493,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -3580,7 +3581,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -3624,7 +3625,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -3668,7 +3669,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -3750,7 +3751,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>73</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -3838,7 +3839,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -3882,7 +3883,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -3923,7 +3924,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -3967,7 +3968,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -4096,7 +4097,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -4178,7 +4179,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>91</v>
       </c>
@@ -4219,7 +4220,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>92</v>
       </c>
@@ -4263,7 +4264,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>93</v>
       </c>
@@ -4307,7 +4308,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>94</v>
       </c>
@@ -4351,7 +4352,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>95</v>
       </c>
@@ -4395,7 +4396,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>96</v>
       </c>
@@ -4436,7 +4437,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>97</v>
       </c>
@@ -4480,7 +4481,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>98</v>
       </c>
@@ -4524,7 +4525,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>99</v>
       </c>
@@ -4568,7 +4569,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>100</v>
       </c>
@@ -4612,7 +4613,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -4656,7 +4657,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>102</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>103</v>
       </c>
@@ -4788,7 +4789,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>106</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>107</v>
       </c>
@@ -4920,7 +4921,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>110</v>
       </c>
@@ -4949,7 +4950,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>111</v>
       </c>
@@ -4990,7 +4991,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>113</v>
       </c>
@@ -5034,7 +5035,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>114</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>115</v>
       </c>
@@ -5116,7 +5117,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>116</v>
       </c>
@@ -5160,7 +5161,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>118</v>
       </c>
@@ -5204,7 +5205,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>119</v>
       </c>
@@ -5245,7 +5246,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>121</v>
       </c>
@@ -5289,7 +5290,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>122</v>
       </c>
@@ -5333,7 +5334,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>123</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>124</v>
       </c>
@@ -5406,7 +5407,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>126</v>
       </c>
@@ -5447,7 +5448,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>127</v>
       </c>
@@ -5491,7 +5492,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>128</v>
       </c>
@@ -5535,7 +5536,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>129</v>
       </c>
@@ -5576,7 +5577,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>130</v>
       </c>
@@ -5620,7 +5621,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>132</v>
       </c>
@@ -5664,7 +5665,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>133</v>
       </c>
@@ -5708,7 +5709,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>134</v>
       </c>
@@ -5749,7 +5750,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>135</v>
       </c>
@@ -5793,7 +5794,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>136</v>
       </c>
@@ -5837,7 +5838,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>138</v>
       </c>
@@ -5875,7 +5876,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>139</v>
       </c>
@@ -5919,7 +5920,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>141</v>
       </c>
@@ -5945,7 +5946,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>142</v>
       </c>
@@ -5983,7 +5984,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -6027,7 +6028,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>144</v>
       </c>
@@ -6071,7 +6072,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>145</v>
       </c>
@@ -6144,7 +6145,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>149</v>
       </c>
@@ -6188,7 +6189,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>151</v>
       </c>
@@ -6232,7 +6233,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>153</v>
       </c>
@@ -6276,7 +6277,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>155</v>
       </c>
@@ -6317,7 +6318,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>156</v>
       </c>
@@ -6358,7 +6359,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>157</v>
       </c>
@@ -6402,7 +6403,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>159</v>
       </c>
@@ -6443,7 +6444,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>160</v>
       </c>
@@ -6487,7 +6488,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>161</v>
       </c>
@@ -6531,7 +6532,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>162</v>
       </c>
@@ -6575,7 +6576,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>163</v>
       </c>
@@ -6616,7 +6617,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>164</v>
       </c>
@@ -6660,7 +6661,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>165</v>
       </c>
@@ -6704,7 +6705,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>166</v>
       </c>
@@ -6748,7 +6749,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>168</v>
       </c>
@@ -6792,7 +6793,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>169</v>
       </c>
@@ -6833,7 +6834,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>170</v>
       </c>
@@ -6874,7 +6875,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>171</v>
       </c>
@@ -6915,7 +6916,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>172</v>
       </c>
@@ -6959,7 +6960,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>173</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>174</v>
       </c>
@@ -7044,7 +7045,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>175</v>
       </c>
@@ -7088,7 +7089,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>176</v>
       </c>
@@ -7114,7 +7115,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>177</v>
       </c>
@@ -7155,7 +7156,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>178</v>
       </c>
@@ -7199,7 +7200,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>180</v>
       </c>
@@ -7243,7 +7244,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>181</v>
       </c>
@@ -7287,7 +7288,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>182</v>
       </c>
@@ -7331,7 +7332,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>184</v>
       </c>
@@ -7372,7 +7373,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>185</v>
       </c>
@@ -7416,7 +7417,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>186</v>
       </c>
@@ -7460,7 +7461,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>187</v>
       </c>
@@ -7504,7 +7505,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>188</v>
       </c>
@@ -7548,7 +7549,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>189</v>
       </c>
@@ -7592,7 +7593,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>191</v>
       </c>
@@ -7636,7 +7637,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>192</v>
       </c>
@@ -7677,7 +7678,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>193</v>
       </c>
@@ -7721,7 +7722,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>194</v>
       </c>
@@ -7762,7 +7763,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>195</v>
       </c>
@@ -7800,7 +7801,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>196</v>
       </c>
@@ -7841,7 +7842,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>198</v>
       </c>
@@ -7882,7 +7883,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>199</v>
       </c>
@@ -7926,7 +7927,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>200</v>
       </c>
@@ -7970,7 +7971,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>202</v>
       </c>
@@ -8014,7 +8015,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>204</v>
       </c>
@@ -8055,7 +8056,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>205</v>
       </c>
@@ -8081,7 +8082,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>206</v>
       </c>
@@ -8125,7 +8126,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>208</v>
       </c>
@@ -8166,7 +8167,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>209</v>
       </c>
@@ -8254,7 +8255,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>211</v>
       </c>
@@ -8298,7 +8299,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>212</v>
       </c>
@@ -8342,7 +8343,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>213</v>
       </c>
@@ -8386,7 +8387,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>214</v>
       </c>
@@ -8427,7 +8428,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>215</v>
       </c>
@@ -8471,7 +8472,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>217</v>
       </c>
@@ -8515,7 +8516,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>219</v>
       </c>
@@ -8556,7 +8557,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>221</v>
       </c>
@@ -8582,7 +8583,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>222</v>
       </c>
@@ -8626,7 +8627,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>223</v>
       </c>
@@ -8667,7 +8668,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>225</v>
       </c>
@@ -8711,7 +8712,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>226</v>
       </c>
@@ -8755,7 +8756,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>227</v>
       </c>
@@ -8796,7 +8797,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>228</v>
       </c>
@@ -8840,7 +8841,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>229</v>
       </c>
@@ -8884,7 +8885,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>230</v>
       </c>
@@ -8922,7 +8923,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>231</v>
       </c>
@@ -8963,7 +8964,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>232</v>
       </c>
@@ -9007,7 +9008,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>233</v>
       </c>
@@ -9048,7 +9049,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>234</v>
       </c>
@@ -9092,7 +9093,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>235</v>
       </c>
@@ -9136,7 +9137,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>236</v>
       </c>
@@ -9180,7 +9181,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>237</v>
       </c>
@@ -9224,7 +9225,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>238</v>
       </c>
@@ -9268,7 +9269,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>239</v>
       </c>
@@ -9312,7 +9313,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>241</v>
       </c>
@@ -9356,7 +9357,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>242</v>
       </c>
@@ -9400,7 +9401,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>243</v>
       </c>
@@ -9444,7 +9445,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>245</v>
       </c>
@@ -9488,7 +9489,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>246</v>
       </c>
@@ -9532,7 +9533,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>247</v>
       </c>
@@ -9573,7 +9574,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>248</v>
       </c>
@@ -9617,7 +9618,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>249</v>
       </c>
@@ -9658,7 +9659,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>250</v>
       </c>
@@ -9702,7 +9703,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>251</v>
       </c>
@@ -9743,7 +9744,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>252</v>
       </c>
@@ -9784,7 +9785,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>253</v>
       </c>
@@ -9828,7 +9829,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>254</v>
       </c>
@@ -9872,7 +9873,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>256</v>
       </c>
@@ -9916,7 +9917,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>257</v>
       </c>
@@ -9942,7 +9943,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>258</v>
       </c>
@@ -9986,7 +9987,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>260</v>
       </c>
@@ -10027,7 +10028,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>261</v>
       </c>
@@ -10071,7 +10072,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>262</v>
       </c>
@@ -10115,7 +10116,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>263</v>
       </c>
@@ -10159,7 +10160,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>264</v>
       </c>
@@ -10203,7 +10204,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>265</v>
       </c>
@@ -10247,7 +10248,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>267</v>
       </c>
@@ -10291,7 +10292,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>268</v>
       </c>
@@ -10332,7 +10333,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>269</v>
       </c>
@@ -10376,7 +10377,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>271</v>
       </c>
@@ -10420,7 +10421,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>272</v>
       </c>
@@ -10464,7 +10465,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>273</v>
       </c>
@@ -10508,7 +10509,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>274</v>
       </c>
@@ -10534,7 +10535,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>275</v>
       </c>
@@ -10575,7 +10576,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>276</v>
       </c>
@@ -10619,7 +10620,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>277</v>
       </c>
@@ -10663,7 +10664,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>278</v>
       </c>
@@ -10707,7 +10708,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>279</v>
       </c>
@@ -10751,7 +10752,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>280</v>
       </c>
@@ -10795,7 +10796,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>281</v>
       </c>
@@ -10836,7 +10837,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>282</v>
       </c>
@@ -10880,7 +10881,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>283</v>
       </c>
@@ -10924,7 +10925,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>284</v>
       </c>
@@ -10965,7 +10966,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>285</v>
       </c>
@@ -11009,7 +11010,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>287</v>
       </c>
@@ -11035,7 +11036,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>288</v>
       </c>
@@ -11079,7 +11080,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>289</v>
       </c>
@@ -11123,7 +11124,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>290</v>
       </c>
@@ -11149,7 +11150,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>291</v>
       </c>
@@ -11193,7 +11194,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>293</v>
       </c>
@@ -11237,7 +11238,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>294</v>
       </c>
@@ -11281,7 +11282,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>295</v>
       </c>
@@ -11325,7 +11326,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>296</v>
       </c>
@@ -11366,7 +11367,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>297</v>
       </c>
@@ -11410,7 +11411,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>298</v>
       </c>
@@ -11454,7 +11455,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>299</v>
       </c>
@@ -11498,7 +11499,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>300</v>
       </c>
@@ -11542,7 +11543,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>301</v>
       </c>
@@ -11583,7 +11584,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>302</v>
       </c>
@@ -11627,7 +11628,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>304</v>
       </c>
@@ -11671,7 +11672,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>305</v>
       </c>
@@ -11715,7 +11716,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>306</v>
       </c>
@@ -11759,7 +11760,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>307</v>
       </c>
@@ -11803,7 +11804,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>308</v>
       </c>
@@ -11847,7 +11848,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>309</v>
       </c>
@@ -11891,7 +11892,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>310</v>
       </c>
@@ -11935,7 +11936,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>311</v>
       </c>
@@ -11979,7 +11980,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>312</v>
       </c>
@@ -12005,7 +12006,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>313</v>
       </c>
@@ -12046,7 +12047,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>314</v>
       </c>
@@ -12090,7 +12091,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>316</v>
       </c>
@@ -12131,7 +12132,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>317</v>
       </c>
@@ -12175,7 +12176,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>318</v>
       </c>
@@ -12216,7 +12217,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>319</v>
       </c>
@@ -12260,7 +12261,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>320</v>
       </c>
@@ -12301,7 +12302,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>321</v>
       </c>
@@ -12345,7 +12346,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>322</v>
       </c>
@@ -12389,7 +12390,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>323</v>
       </c>
@@ -12433,7 +12434,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>325</v>
       </c>
@@ -12477,7 +12478,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>326</v>
       </c>
@@ -12521,7 +12522,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>327</v>
       </c>
@@ -12565,7 +12566,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>329</v>
       </c>
@@ -12609,7 +12610,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>330</v>
       </c>
@@ -12653,7 +12654,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>332</v>
       </c>
@@ -12694,7 +12695,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>333</v>
       </c>
@@ -12738,7 +12739,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>335</v>
       </c>
@@ -12782,7 +12783,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>336</v>
       </c>
@@ -12826,7 +12827,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>337</v>
       </c>
@@ -12867,7 +12868,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>338</v>
       </c>
@@ -12911,7 +12912,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>339</v>
       </c>
@@ -12955,7 +12956,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>341</v>
       </c>
@@ -12999,7 +13000,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>343</v>
       </c>
@@ -13043,7 +13044,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>344</v>
       </c>
@@ -13087,7 +13088,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>346</v>
       </c>
@@ -13131,7 +13132,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>347</v>
       </c>
@@ -13175,7 +13176,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>348</v>
       </c>
@@ -13219,7 +13220,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>349</v>
       </c>
@@ -13263,7 +13264,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>350</v>
       </c>
@@ -13307,7 +13308,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>351</v>
       </c>
@@ -13348,7 +13349,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>352</v>
       </c>
@@ -13392,7 +13393,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>354</v>
       </c>
@@ -13436,7 +13437,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>355</v>
       </c>
@@ -13480,7 +13481,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>356</v>
       </c>
@@ -13524,7 +13525,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>358</v>
       </c>
@@ -13550,7 +13551,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>359</v>
       </c>
@@ -13594,7 +13595,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>361</v>
       </c>
@@ -13635,7 +13636,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>362</v>
       </c>
@@ -13679,7 +13680,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>364</v>
       </c>
@@ -13723,7 +13724,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>366</v>
       </c>
@@ -13767,7 +13768,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>367</v>
       </c>
@@ -13811,7 +13812,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>368</v>
       </c>
@@ -13855,7 +13856,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>369</v>
       </c>
@@ -13899,7 +13900,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>370</v>
       </c>
@@ -13943,7 +13944,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>372</v>
       </c>
@@ -13984,7 +13985,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>374</v>
       </c>
@@ -14028,7 +14029,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>375</v>
       </c>
@@ -14072,7 +14073,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>377</v>
       </c>
@@ -14116,7 +14117,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>378</v>
       </c>
@@ -14157,7 +14158,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>379</v>
       </c>
@@ -14201,7 +14202,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>380</v>
       </c>
@@ -14245,7 +14246,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>381</v>
       </c>
@@ -14289,7 +14290,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>382</v>
       </c>
@@ -14333,7 +14334,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>383</v>
       </c>
@@ -14377,7 +14378,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>384</v>
       </c>
@@ -14421,7 +14422,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>385</v>
       </c>
@@ -14465,7 +14466,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>387</v>
       </c>
@@ -14506,7 +14507,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>389</v>
       </c>
@@ -14547,7 +14548,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>390</v>
       </c>
@@ -14591,7 +14592,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>392</v>
       </c>
@@ -14632,7 +14633,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>393</v>
       </c>
@@ -14676,7 +14677,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>394</v>
       </c>
@@ -14720,7 +14721,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>395</v>
       </c>
@@ -14764,7 +14765,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>396</v>
       </c>
@@ -14808,7 +14809,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>397</v>
       </c>
@@ -14849,7 +14850,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>398</v>
       </c>
@@ -14893,7 +14894,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>399</v>
       </c>
@@ -14934,7 +14935,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="309" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>400</v>
       </c>
@@ -14960,7 +14961,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>401</v>
       </c>
@@ -15001,7 +15002,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="311" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>402</v>
       </c>
@@ -15045,7 +15046,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>403</v>
       </c>
@@ -15089,7 +15090,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>404</v>
       </c>
@@ -15133,7 +15134,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="314" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>405</v>
       </c>
@@ -15174,7 +15175,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="315" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>406</v>
       </c>
@@ -15218,7 +15219,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="316" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>407</v>
       </c>
@@ -15262,7 +15263,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="317" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>409</v>
       </c>
@@ -15350,7 +15351,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="319" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>412</v>
       </c>
@@ -15391,7 +15392,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="320" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>413</v>
       </c>
@@ -15435,7 +15436,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="321" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>414</v>
       </c>
@@ -15479,7 +15480,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="322" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>415</v>
       </c>
@@ -15523,7 +15524,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="323" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>416</v>
       </c>
@@ -15549,7 +15550,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="324" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>417</v>
       </c>
@@ -15593,7 +15594,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="325" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>418</v>
       </c>
@@ -15637,7 +15638,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="326" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>419</v>
       </c>
@@ -15681,7 +15682,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="327" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>421</v>
       </c>
@@ -15725,7 +15726,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="328" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>422</v>
       </c>
@@ -15769,7 +15770,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>423</v>
       </c>
@@ -15813,7 +15814,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="330" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>424</v>
       </c>
@@ -15854,7 +15855,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>425</v>
       </c>
@@ -15898,7 +15899,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="332" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>426</v>
       </c>
@@ -15942,7 +15943,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="333" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>427</v>
       </c>
@@ -15986,7 +15987,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="334" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>428</v>
       </c>
@@ -16027,7 +16028,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="335" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>429</v>
       </c>
@@ -16071,7 +16072,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="336" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>431</v>
       </c>
@@ -16115,7 +16116,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="337" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>432</v>
       </c>
@@ -16159,7 +16160,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="338" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>433</v>
       </c>
@@ -16203,7 +16204,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="339" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>435</v>
       </c>
@@ -16244,7 +16245,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="340" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>436</v>
       </c>
@@ -16288,7 +16289,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="341" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>437</v>
       </c>
@@ -16332,7 +16333,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="342" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>438</v>
       </c>
@@ -16373,7 +16374,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="343" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>439</v>
       </c>
@@ -16399,7 +16400,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="344" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>440</v>
       </c>
@@ -16443,7 +16444,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="345" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>442</v>
       </c>
@@ -16484,7 +16485,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="346" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>443</v>
       </c>
@@ -16528,7 +16529,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="347" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>444</v>
       </c>
@@ -16572,7 +16573,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="348" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>445</v>
       </c>
@@ -16616,7 +16617,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="349" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>446</v>
       </c>
@@ -16660,7 +16661,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="350" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>447</v>
       </c>
@@ -16704,7 +16705,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="351" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>448</v>
       </c>
@@ -16745,7 +16746,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="352" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>449</v>
       </c>
@@ -16786,7 +16787,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="353" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>450</v>
       </c>
@@ -16827,7 +16828,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="354" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>451</v>
       </c>
@@ -16868,7 +16869,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="355" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>453</v>
       </c>
@@ -16912,7 +16913,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="356" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>454</v>
       </c>
@@ -16956,7 +16957,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="357" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>455</v>
       </c>
@@ -17000,7 +17001,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="358" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>456</v>
       </c>
@@ -17041,7 +17042,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="359" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>458</v>
       </c>
@@ -17085,7 +17086,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="360" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>459</v>
       </c>
@@ -17129,7 +17130,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="361" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>460</v>
       </c>
@@ -17170,7 +17171,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="362" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>462</v>
       </c>
@@ -17214,7 +17215,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="363" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>464</v>
       </c>
@@ -17258,7 +17259,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="364" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>465</v>
       </c>
@@ -17287,7 +17288,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="365" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>466</v>
       </c>
@@ -17331,7 +17332,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="366" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>467</v>
       </c>
@@ -17375,7 +17376,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="367" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>468</v>
       </c>
@@ -17404,7 +17405,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="368" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>469</v>
       </c>
@@ -17448,7 +17449,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="369" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>471</v>
       </c>
@@ -17492,7 +17493,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>473</v>
       </c>
@@ -17536,7 +17537,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>474</v>
       </c>
@@ -17577,7 +17578,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>475</v>
       </c>
@@ -17621,7 +17622,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>477</v>
       </c>
@@ -17662,7 +17663,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>478</v>
       </c>
@@ -17706,7 +17707,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="375" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>479</v>
       </c>
@@ -17747,7 +17748,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>480</v>
       </c>
@@ -17791,7 +17792,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="377" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>481</v>
       </c>
@@ -17835,7 +17836,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="378" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>482</v>
       </c>
@@ -17879,7 +17880,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="379" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>483</v>
       </c>
@@ -17905,7 +17906,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="380" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>484</v>
       </c>
@@ -17946,7 +17947,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="381" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>485</v>
       </c>
@@ -17990,7 +17991,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="382" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>486</v>
       </c>
@@ -18019,7 +18020,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="383" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>487</v>
       </c>
@@ -18063,7 +18064,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>488</v>
       </c>
@@ -18107,7 +18108,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>489</v>
       </c>
@@ -18136,7 +18137,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>490</v>
       </c>
@@ -18180,7 +18181,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>491</v>
       </c>
@@ -18221,7 +18222,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>492</v>
       </c>
@@ -18262,7 +18263,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>493</v>
       </c>
@@ -18303,7 +18304,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>494</v>
       </c>
@@ -18347,7 +18348,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="391" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>496</v>
       </c>
@@ -18391,7 +18392,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="392" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>497</v>
       </c>
@@ -18435,7 +18436,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="393" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>498</v>
       </c>
@@ -18479,7 +18480,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="394" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>499</v>
       </c>
@@ -18524,7 +18525,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N393" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:N394" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="12">
+      <filters>
+        <filter val="Aurora"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se actualizo una metrica
</commit_message>
<xml_diff>
--- a/uploads/metricas_2025-07.xlsx
+++ b/uploads/metricas_2025-07.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arg_2\OneDrive\Escritorio\Dashboard\SonarQube\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA532DE-651F-4268-BB67-EF18B7E4291F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B07A7CD-2D5D-4BFC-9109-892CB586FB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="384" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2908" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2907" uniqueCount="500">
   <si>
     <t>NombreProyecto</t>
   </si>
@@ -1895,8 +1895,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N394"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A394" sqref="A394"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L203" sqref="L203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2403,7 +2403,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>105</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>109</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>147</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>210</v>
       </c>
@@ -10421,7 +10421,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>272</v>
       </c>
@@ -10434,11 +10434,11 @@
       <c r="D203" t="s">
         <v>15</v>
       </c>
-      <c r="E203" t="s">
-        <v>16</v>
+      <c r="E203">
+        <v>76</v>
       </c>
       <c r="F203" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G203">
         <v>0</v>
@@ -15307,7 +15307,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>411</v>
       </c>
@@ -18526,9 +18526,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N394" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="12">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Aurora"/>
+        <filter val="AEL.ControlAcceso.Servicio:Quality"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>